<commit_message>
Carga completa de mayo
</commit_message>
<xml_diff>
--- a/dags/files_pami/Enfermeria.xlsx
+++ b/dags/files_pami/Enfermeria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clinicossasips-my.sharepoint.com/personal/maristizabal_clinicos_com_co/Documents/GESTIÓN DE TABLEROS/ACTUALIZACION PAMI Y CARTAGENA/ENFERMERIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{5DBBA766-86D2-44AC-B8A2-89A14182EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98A3AA28-D210-4E41-AAFE-574DCF3F991A}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{5DBBA766-86D2-44AC-B8A2-89A14182EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{105D3F8B-1B06-4809-89F7-049959F28231}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7808414F-6824-43BD-9124-FFAD4C1019A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7808414F-6824-43BD-9124-FFAD4C1019A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>Sede</t>
   </si>
@@ -242,8 +242,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B921363-6047-4765-A590-AD9805DC5954}" name="Tabla1" displayName="Tabla1" ref="A1:D20" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:D20" xr:uid="{7B921363-6047-4765-A590-AD9805DC5954}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B921363-6047-4765-A590-AD9805DC5954}" name="Tabla1" displayName="Tabla1" ref="A1:D19" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:D19" xr:uid="{7B921363-6047-4765-A590-AD9805DC5954}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4197E606-E0B2-46B1-9FC8-D6E5223FCD33}" name="Sede"/>
     <tableColumn id="2" xr3:uid="{4FD07CCA-7C56-4E42-BEA1-E6992E7CF17E}" name="Mes" dataDxfId="0"/>
@@ -551,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86D84D7-304C-4227-9493-2AF1EA3A1C73}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,13 +584,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>130</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -598,13 +598,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>188</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -612,13 +612,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,7 +626,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -640,13 +640,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -654,13 +654,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -668,13 +668,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,13 +682,13 @@
         <v>16</v>
       </c>
       <c r="B9" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9">
-        <v>70</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,13 +696,13 @@
         <v>16</v>
       </c>
       <c r="B10" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -710,7 +710,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -724,7 +724,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -738,13 +738,13 @@
         <v>16</v>
       </c>
       <c r="B13" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13">
-        <v>161</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -752,7 +752,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -766,13 +766,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -780,13 +780,13 @@
         <v>17</v>
       </c>
       <c r="B16" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -794,13 +794,13 @@
         <v>17</v>
       </c>
       <c r="B17" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -822,27 +822,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
       <c r="D19">
         <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="1">
-        <v>44986</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1034,13 +1020,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3838589E-B9FB-4787-AF1E-425AABB6AC4E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A182C52F-7258-4BA3-8E0B-2AE7EABB1688}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8361DF0D-89F1-49FB-B846-9E3771EA8E32}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8665E59D-99D2-434A-9674-2331B6FF6BBE}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE5C3D2E-C11F-466A-9360-816D8C84946B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBC368A2-9C83-47E2-A9CB-147CD5E1DF97}"/>
 </file>
</xml_diff>

<commit_message>
Cambios en domiciliaria y PAMI
</commit_message>
<xml_diff>
--- a/dags/files_pami/Enfermeria.xlsx
+++ b/dags/files_pami/Enfermeria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clinicossasips-my.sharepoint.com/personal/maristizabal_clinicos_com_co/Documents/GESTIÓN DE TABLEROS/ACTUALIZACION PAMI Y CARTAGENA/ENFERMERIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{5DBBA766-86D2-44AC-B8A2-89A14182EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{105D3F8B-1B06-4809-89F7-049959F28231}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="8_{5DBBA766-86D2-44AC-B8A2-89A14182EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A165CF1E-6398-4FC4-B57A-14FC27D3D0A8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7808414F-6824-43BD-9124-FFAD4C1019A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>Sede</t>
   </si>
@@ -59,37 +59,31 @@
     <t>TOMA DE EKG</t>
   </si>
   <si>
-    <t>LAVADO DE OIDO</t>
-  </si>
-  <si>
     <t>RETIRO DE PUNTOS</t>
   </si>
   <si>
-    <t>CURACION</t>
-  </si>
-  <si>
     <t>TOMA DE TENSÓN ARTERIAL</t>
   </si>
   <si>
-    <t>INYECTOLOGIA</t>
-  </si>
-  <si>
-    <t>LAVADO DE OIDOS</t>
-  </si>
-  <si>
-    <t>GLUCOMETRIA</t>
-  </si>
-  <si>
     <t xml:space="preserve">TOMA DE EKG </t>
   </si>
   <si>
-    <t>TOMA DE TENSION ARTERIAL</t>
-  </si>
-  <si>
     <t>San Martin</t>
   </si>
   <si>
     <t>Cartagena</t>
+  </si>
+  <si>
+    <t>LAVADO DE OÍDOS</t>
+  </si>
+  <si>
+    <t>CURACIÓN</t>
+  </si>
+  <si>
+    <t>TOMA DE TENSIÓN ARTERIAL</t>
+  </si>
+  <si>
+    <t>GLUCOMETRÍA</t>
   </si>
 </sst>
 </file>
@@ -553,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86D84D7-304C-4227-9493-2AF1EA3A1C73}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -584,13 +578,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>99</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -598,13 +592,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -612,13 +606,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,13 +620,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -640,13 +634,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -654,13 +648,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -668,167 +662,167 @@
         <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>60</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13">
-        <v>123</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D17">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B18" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1013,20 +1007,10 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A182C52F-7258-4BA3-8E0B-2AE7EABB1688}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD7AF7FE-9FDF-4DC8-AE4E-2E64D6243290}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8665E59D-99D2-434A-9674-2331B6FF6BBE}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBC368A2-9C83-47E2-A9CB-147CD5E1DF97}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48E8B2D8-7C8C-4492-A456-9E7B070257F2}"/>
 </file>
</xml_diff>

<commit_message>
commit de actualizacion 18-08-2023 57 archivos
</commit_message>
<xml_diff>
--- a/dags/files_pami/Enfermeria.xlsx
+++ b/dags/files_pami/Enfermeria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clinicossasips-my.sharepoint.com/personal/maristizabal_clinicos_com_co/Documents/GESTIÓN DE TABLEROS/ACTUALIZACION PAMI Y CARTAGENA/ENFERMERIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{5DBBA766-86D2-44AC-B8A2-89A14182EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55D17549-FF81-4F82-B4D4-1CD8999632A0}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{5DBBA766-86D2-44AC-B8A2-89A14182EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF417052-AFD8-4C50-9642-453FFAC5ED9E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7808414F-6824-43BD-9124-FFAD4C1019A8}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,13 +578,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -592,13 +592,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>152</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -606,13 +606,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -620,13 +620,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -634,13 +634,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -648,13 +648,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -662,13 +662,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -676,13 +676,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -690,13 +690,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -704,7 +704,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -718,13 +718,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12">
-        <v>81</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -732,13 +732,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -746,13 +746,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -760,13 +760,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -774,13 +774,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -788,13 +788,13 @@
         <v>11</v>
       </c>
       <c r="B17" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17">
-        <v>97</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -802,13 +802,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18">
-        <v>96</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -816,13 +816,13 @@
         <v>11</v>
       </c>
       <c r="B19" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -830,13 +830,13 @@
         <v>11</v>
       </c>
       <c r="B20" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="1">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
@@ -862,8 +862,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E8AAD53D957193499A95B0822EE92604" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="33b02bf87a1dd6f4b3a4b5e0f725ed7a">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b848449e-c9d3-4969-a575-ff0d96471e4b" xmlns:ns3="ac8deb47-86bc-4260-8fcd-a6158e6e95f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f6d66165c6d3d4cf8e0bc57ff34d5fa9" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E8AAD53D957193499A95B0822EE92604" ma:contentTypeVersion="5" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="64521337f70ab7452aeeac0760611e10">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b848449e-c9d3-4969-a575-ff0d96471e4b" xmlns:ns3="ac8deb47-86bc-4260-8fcd-a6158e6e95f4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bab967c49d094239a50a0e5887e9ad5e" ns2:_="" ns3:_="">
     <xsd:import namespace="b848449e-c9d3-4969-a575-ff0d96471e4b"/>
     <xsd:import namespace="ac8deb47-86bc-4260-8fcd-a6158e6e95f4"/>
     <xsd:element name="properties">
@@ -876,6 +876,7 @@
                 <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -924,6 +925,11 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1036,9 +1042,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFEA1F8A-93FA-434C-A356-1051DBDED129}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24BA2AF2-3A64-4EDA-B297-3C86AFCABCA0}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9723CBD6-2932-48F8-BAAE-23592FB16900}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71E0D9D8-28F7-472F-BA68-B333F60D2014}"/>
 </file>
</xml_diff>

<commit_message>
update many dags --NEPS --Masiva --MasivaCompensar
</commit_message>
<xml_diff>
--- a/dags/files_pami/Enfermeria.xlsx
+++ b/dags/files_pami/Enfermeria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clinicossasips-my.sharepoint.com/personal/maristizabal_clinicos_com_co/Documents/GESTIÓN DE TABLEROS/ACTUALIZACION PAMI Y CARTAGENA/ENFERMERIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="8_{5DBBA766-86D2-44AC-B8A2-89A14182EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B84764F-8E18-4A9E-A7A6-C2332C77A236}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{5DBBA766-86D2-44AC-B8A2-89A14182EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA76F823-3946-44D8-9D67-B1C10B1A579D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7808414F-6824-43BD-9124-FFAD4C1019A8}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,13 +578,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -592,13 +592,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -606,13 +606,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -620,13 +620,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -634,13 +634,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -648,27 +648,27 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -676,13 +676,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D9">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -690,13 +690,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -704,13 +704,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11">
-        <v>146</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -718,13 +718,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -732,13 +732,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -746,13 +746,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -760,13 +760,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -774,13 +774,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -788,7 +788,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -802,13 +802,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -816,13 +816,13 @@
         <v>11</v>
       </c>
       <c r="B19" s="1">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1014,9 +1014,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71667CAF-757F-4C4E-A74A-250CDC082421}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63D481FD-452A-4436-80D4-6D6D18A3B06D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{689191D6-E07C-47B7-91AE-EC9BC022013B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE6A6AEE-C335-4917-94AD-E52376ACA844}"/>
 </file>
</xml_diff>

<commit_message>
Cambios a noviembre 20 2023
</commit_message>
<xml_diff>
--- a/dags/files_pami/Enfermeria.xlsx
+++ b/dags/files_pami/Enfermeria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clinicossasips-my.sharepoint.com/personal/maristizabal_clinicos_com_co/Documents/GESTIÓN DE TABLEROS/ACTUALIZACION PAMI Y CARTAGENA/ENFERMERIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="8_{5DBBA766-86D2-44AC-B8A2-89A14182EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA76F823-3946-44D8-9D67-B1C10B1A579D}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="8_{5DBBA766-86D2-44AC-B8A2-89A14182EAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16FBBA9E-46A0-4E6A-A2FF-7E4EEFB81882}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7808414F-6824-43BD-9124-FFAD4C1019A8}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>RETIRO DE PUNTOS</t>
   </si>
   <si>
-    <t>TOMA DE TENSÓN ARTERIAL</t>
-  </si>
-  <si>
     <t xml:space="preserve">TOMA DE EKG </t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>GLUCOMETRÍA</t>
+  </si>
+  <si>
+    <t>LAVADO NASAL</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86D84D7-304C-4227-9493-2AF1EA3A1C73}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,13 +578,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>84</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -592,13 +592,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -606,13 +606,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -620,13 +620,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -634,13 +634,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -648,94 +648,94 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>89</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>147</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -743,86 +743,86 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D14">
-        <v>90</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
         <v>6</v>
-      </c>
-      <c r="D15">
-        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D16">
-        <v>110</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1014,9 +1014,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63D481FD-452A-4436-80D4-6D6D18A3B06D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6683D252-034C-439B-AF23-6E7CD04AF4A0}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE6A6AEE-C335-4917-94AD-E52376ACA844}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51CB9817-D56F-47D1-93BC-7DD6CCC72078}"/>
 </file>
</xml_diff>